<commit_message>
added new test cases for specific user
Added new test cases for Karancsi Matyas.
</commit_message>
<xml_diff>
--- a/test_log.xlsx
+++ b/test_log.xlsx
@@ -1,22 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karan\Documents\GitHub\SzoftverfejlesztesModszertanMiniProject\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE9469EF-6B91-4938-8252-169392434C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Export Summary" sheetId="1" r:id="rId4"/>
-    <sheet name="test_DB" sheetId="2" r:id="rId5"/>
-    <sheet name="test_MB" sheetId="3" r:id="rId6"/>
-    <sheet name="test_VN" sheetId="4" r:id="rId7"/>
-    <sheet name="test_KM" sheetId="5" r:id="rId8"/>
-    <sheet name="test_SZ" sheetId="6" r:id="rId9"/>
+    <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
+    <sheet name="test_DB" sheetId="2" r:id="rId2"/>
+    <sheet name="test_MB" sheetId="3" r:id="rId3"/>
+    <sheet name="test_VN" sheetId="4" r:id="rId4"/>
+    <sheet name="test_KM" sheetId="5" r:id="rId5"/>
+    <sheet name="test_SZ" sheetId="6" r:id="rId6"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="77">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -232,20 +241,39 @@
   </si>
   <si>
     <t>Server redirects to the Dashboard</t>
+  </si>
+  <si>
+    <t>Send a post request to the server with username, email, password. Incorrect credentials</t>
+  </si>
+  <si>
+    <t>User clicks on like button</t>
+  </si>
+  <si>
+    <t>Number of likes are increased</t>
+  </si>
+  <si>
+    <t>User clicks on dislike button</t>
+  </si>
+  <si>
+    <t>Number of dislikes are increased</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -258,23 +286,13 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <u val="single"/>
+      <u/>
       <sz val="12"/>
       <color indexed="11"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="15"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
@@ -285,7 +303,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -320,6 +338,18 @@
       <patternFill patternType="solid">
         <fgColor indexed="20"/>
         <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -467,107 +497,119 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="34">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="30">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="14"/>
+          <bgColor indexed="16"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -640,47 +682,89 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="14"/>
-          <bgColor indexed="16"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ff5e88b1"/>
-      <rgbColor rgb="ffeef3f4"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FF5E88B1"/>
+      <rgbColor rgb="FFEEF3F4"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
       <rgbColor rgb="00000000"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff92d050"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
-      <rgbColor rgb="ff111111"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF92D050"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="FF111111"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office-téma">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-téma">
   <a:themeElements>
     <a:clrScheme name="Office-téma">
       <a:dk1>
@@ -882,7 +966,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -900,7 +984,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -929,7 +1013,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -954,7 +1038,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -979,7 +1063,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1004,7 +1088,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1029,7 +1113,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1054,7 +1138,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1079,7 +1163,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1104,7 +1188,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1129,7 +1213,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1142,9 +1226,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1161,7 +1251,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1179,7 +1269,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1204,7 +1294,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1229,7 +1319,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1254,7 +1344,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1279,7 +1369,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1304,7 +1394,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1329,7 +1419,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1354,7 +1444,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1379,7 +1469,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1404,7 +1494,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1417,9 +1507,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1433,7 +1529,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1451,7 +1547,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1480,7 +1576,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1505,7 +1601,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1530,7 +1626,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1555,7 +1651,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1580,7 +1676,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1605,7 +1701,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1630,7 +1726,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1655,7 +1751,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1680,7 +1776,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1693,122 +1789,132 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B3:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.95" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="4" width="30.5547" customWidth="1"/>
+    <col min="2" max="4" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" ht="0.05" customHeight="1">
-      <c r="B3" t="s" s="1">
+    <row r="3" spans="2:4" ht="0" hidden="1" customHeight="1">
+      <c r="B3" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C3"/>
-      <c r="D3"/>
-    </row>
-    <row r="7">
-      <c r="B7" t="s" s="2">
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+    </row>
+    <row r="7" spans="2:4" ht="18.75">
+      <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C7" t="s" s="2">
+      <c r="C7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D7" t="s" s="2">
+      <c r="D7" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9">
-      <c r="B9" t="s" s="3">
+    <row r="9" spans="2:4" ht="15.75">
+      <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10">
-      <c r="B10" s="4"/>
-      <c r="C10" t="s" s="4">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="2:4" ht="15.75">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D10" t="s" s="5">
+      <c r="D10" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11">
-      <c r="B11" t="s" s="3">
+    <row r="11" spans="2:4" ht="15.75">
+      <c r="B11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12">
-      <c r="B12" s="4"/>
-      <c r="C12" t="s" s="4">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="2:4" ht="15.75">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D12" t="s" s="5">
+      <c r="D12" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13">
-      <c r="B13" t="s" s="3">
+    <row r="13" spans="2:4" ht="15.75">
+      <c r="B13" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14">
-      <c r="B14" s="4"/>
-      <c r="C14" t="s" s="4">
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="2:4" ht="15.75">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D14" t="s" s="5">
+      <c r="D14" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15">
-      <c r="B15" t="s" s="3">
+    <row r="15" spans="2:4" ht="15.75">
+      <c r="B15" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16">
-      <c r="B16" s="4"/>
-      <c r="C16" t="s" s="4">
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="2:4" ht="15.75">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D16" t="s" s="5">
+      <c r="D16" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17">
-      <c r="B17" t="s" s="3">
+    <row r="17" spans="2:4" ht="15.75">
+      <c r="B17" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18">
-      <c r="B18" s="4"/>
-      <c r="C18" t="s" s="4">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="2:4" ht="15.75">
+      <c r="B18" s="3"/>
+      <c r="C18" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D18" t="s" s="5">
+      <c r="D18" s="4" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1817,184 +1923,186 @@
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D10" location="'test_DB'!R1C1" tooltip="" display="test_DB"/>
-    <hyperlink ref="D12" location="'test_MB'!R1C1" tooltip="" display="test_MB"/>
-    <hyperlink ref="D14" location="'test_VN'!R1C1" tooltip="" display="test_VN"/>
-    <hyperlink ref="D16" location="'test_KM'!R1C1" tooltip="" display="test_KM"/>
-    <hyperlink ref="D18" location="'test_SZ'!R1C1" tooltip="" display="test_SZ"/>
+    <hyperlink ref="D10" location="'test_DB'!R1C1" display="test_DB" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D12" location="'test_MB'!R1C1" display="test_MB" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D14" location="'test_VN'!R1C1" display="test_VN" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D16" location="'test_KM'!R1C1" display="test_KM" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D18" location="'test_SZ'!R1C1" display="test_SZ" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
   </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="9" style="6" customWidth="1"/>
-    <col min="2" max="2" width="20.5" style="6" customWidth="1"/>
-    <col min="3" max="3" width="6.85156" style="6" customWidth="1"/>
-    <col min="4" max="4" width="18.3516" style="6" customWidth="1"/>
-    <col min="5" max="5" width="19.5" style="6" customWidth="1"/>
-    <col min="6" max="6" width="15.6719" style="6" customWidth="1"/>
-    <col min="7" max="16384" width="8.85156" style="6" customWidth="1"/>
+    <col min="1" max="1" width="9" style="5" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="7">
+    <row r="1" spans="1:6" ht="13.5" customHeight="1">
+      <c r="A1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="9"/>
-    </row>
-    <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="7">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="27"/>
+    </row>
+    <row r="2" spans="1:6" ht="13.5" customHeight="1">
+      <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s" s="10">
+      <c r="B2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s" s="10">
+      <c r="C2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s" s="10">
+      <c r="D2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s" s="10">
+      <c r="E2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s" s="7">
+      <c r="F2" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" ht="63" customHeight="1">
-      <c r="A3" t="s" s="7">
+    <row r="3" spans="1:6" ht="63" customHeight="1">
+      <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s" s="11">
+      <c r="B3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s" s="10">
+      <c r="C3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s" s="11">
+      <c r="D3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s" s="11">
+      <c r="E3" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s" s="7">
+      <c r="F3" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" ht="57.75" customHeight="1">
-      <c r="A4" s="9"/>
-      <c r="B4" t="s" s="11">
+    <row r="4" spans="1:6" ht="57.75" customHeight="1">
+      <c r="A4" s="8"/>
+      <c r="B4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s" s="10">
+      <c r="C4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D4" t="s" s="11">
+      <c r="D4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E4" t="s" s="11">
+      <c r="E4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F4" t="s" s="7">
+      <c r="F4" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" ht="28.8" customHeight="1">
-      <c r="A5" t="s" s="7">
+    <row r="5" spans="1:6" ht="28.9" customHeight="1">
+      <c r="A5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B5" t="s" s="11">
+      <c r="B5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C5" t="s" s="10">
+      <c r="C5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D5" t="s" s="11">
+      <c r="D5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E5" t="s" s="11">
+      <c r="E5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F5" t="s" s="7">
+      <c r="F5" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" ht="60" customHeight="1">
-      <c r="A6" s="9"/>
-      <c r="B6" t="s" s="11">
+    <row r="6" spans="1:6" ht="60" customHeight="1">
+      <c r="A6" s="8"/>
+      <c r="B6" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C6" t="s" s="10">
+      <c r="C6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D6" t="s" s="11">
+      <c r="D6" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E6" t="s" s="11">
+      <c r="E6" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F6" t="s" s="7">
+      <c r="F6" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="9"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="9"/>
-    </row>
-    <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="9"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="9"/>
-    </row>
-    <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="9"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="9"/>
-    </row>
-    <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="9"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="9"/>
+    <row r="7" spans="1:6" ht="13.5" customHeight="1">
+      <c r="A7" s="8"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" spans="1:6" ht="13.5" customHeight="1">
+      <c r="A8" s="8"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:6" ht="13.5" customHeight="1">
+      <c r="A9" s="8"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="1:6" ht="13.5" customHeight="1">
+      <c r="A10" s="8"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:C6 D9:D10">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal" stopIfTrue="1">
+    <cfRule type="cellIs" dxfId="9" priority="1" stopIfTrue="1" operator="equal">
       <formula>"failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal" stopIfTrue="1">
+    <cfRule type="cellIs" dxfId="8" priority="2" stopIfTrue="1" operator="equal">
       <formula>"passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -2002,173 +2110,173 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="9" style="13" customWidth="1"/>
-    <col min="2" max="2" width="28.5" style="13" customWidth="1"/>
-    <col min="3" max="3" width="6.85156" style="13" customWidth="1"/>
-    <col min="4" max="4" width="14.5" style="13" customWidth="1"/>
-    <col min="5" max="5" width="11.8516" style="13" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="13" customWidth="1"/>
-    <col min="7" max="7" width="8.85156" style="13" customWidth="1"/>
-    <col min="8" max="16384" width="8.85156" style="13" customWidth="1"/>
+    <col min="1" max="1" width="9" style="5" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="5" customWidth="1"/>
+    <col min="7" max="8" width="8.85546875" style="5" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="10">
+    <row r="1" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A1" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-    </row>
-    <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="10">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+    </row>
+    <row r="2" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s" s="10">
+      <c r="B2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s" s="10">
+      <c r="C2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s" s="10">
+      <c r="D2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s" s="10">
+      <c r="E2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s" s="10">
+      <c r="F2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="12"/>
-    </row>
-    <row r="3" ht="45" customHeight="1">
-      <c r="A3" t="s" s="10">
+      <c r="G2" s="11"/>
+    </row>
+    <row r="3" spans="1:7" ht="45" customHeight="1">
+      <c r="A3" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B3" t="s" s="11">
+      <c r="B3" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C3" t="s" s="10">
+      <c r="C3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s" s="11">
+      <c r="D3" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E3" t="s" s="11">
+      <c r="E3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F3" t="s" s="10">
+      <c r="F3" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="12"/>
-    </row>
-    <row r="4" ht="54" customHeight="1">
-      <c r="A4" s="8"/>
-      <c r="B4" t="s" s="11">
+      <c r="G3" s="11"/>
+    </row>
+    <row r="4" spans="1:7" ht="54" customHeight="1">
+      <c r="A4" s="7"/>
+      <c r="B4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C4" t="s" s="10">
+      <c r="C4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D4" t="s" s="11">
+      <c r="D4" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E4" t="s" s="11">
+      <c r="E4" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="F4" t="s" s="10">
+      <c r="F4" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="12"/>
-    </row>
-    <row r="5" ht="47.4" customHeight="1">
-      <c r="A5" s="8"/>
-      <c r="B5" t="s" s="11">
+      <c r="G4" s="11"/>
+    </row>
+    <row r="5" spans="1:7" ht="47.45" customHeight="1">
+      <c r="A5" s="7"/>
+      <c r="B5" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C5" t="s" s="10">
+      <c r="C5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D5" t="s" s="11">
+      <c r="D5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E5" t="s" s="11">
+      <c r="E5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F5" t="s" s="10">
+      <c r="F5" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="12"/>
-    </row>
-    <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-    </row>
-    <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-    </row>
-    <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-    </row>
-    <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-    </row>
-    <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
+      <c r="G5" s="11"/>
+    </row>
+    <row r="6" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+    </row>
+    <row r="7" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+    </row>
+    <row r="8" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+    </row>
+    <row r="9" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+    </row>
+    <row r="10" spans="1:7" ht="13.5" customHeight="1">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:C5">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal" stopIfTrue="1">
+    <cfRule type="cellIs" dxfId="7" priority="1" stopIfTrue="1" operator="equal">
       <formula>"failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal" stopIfTrue="1">
+    <cfRule type="cellIs" dxfId="6" priority="2" stopIfTrue="1" operator="equal">
       <formula>"passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -2176,210 +2284,210 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.1667" defaultRowHeight="55.8" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="55.9" customHeight="1"/>
   <cols>
-    <col min="1" max="6" width="15.1719" style="14" customWidth="1"/>
-    <col min="7" max="16384" width="15.1719" style="14" customWidth="1"/>
+    <col min="1" max="7" width="15.140625" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="15.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" ht="55.8" customHeight="1">
-      <c r="A1" t="s" s="10">
+    <row r="1" spans="1:6" ht="55.9" customHeight="1">
+      <c r="A1" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-    </row>
-    <row r="2" ht="55.8" customHeight="1">
-      <c r="A2" t="s" s="10">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+    </row>
+    <row r="2" spans="1:6" ht="55.9" customHeight="1">
+      <c r="A2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s" s="10">
+      <c r="B2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s" s="10">
+      <c r="C2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s" s="10">
+      <c r="D2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s" s="10">
+      <c r="E2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s" s="10">
+      <c r="F2" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" ht="55.8" customHeight="1">
-      <c r="A3" s="8"/>
-      <c r="B3" t="s" s="11">
+    <row r="3" spans="1:6" ht="55.9" customHeight="1">
+      <c r="A3" s="7"/>
+      <c r="B3" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C3" t="s" s="10">
+      <c r="C3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D3" t="s" s="11">
+      <c r="D3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E3" t="s" s="11">
+      <c r="E3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F3" t="s" s="10">
+      <c r="F3" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" ht="55.8" customHeight="1">
-      <c r="A4" s="8"/>
-      <c r="B4" t="s" s="11">
+    <row r="4" spans="1:6" ht="55.9" customHeight="1">
+      <c r="A4" s="7"/>
+      <c r="B4" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C4" t="s" s="10">
+      <c r="C4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D4" t="s" s="11">
+      <c r="D4" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E4" t="s" s="11">
+      <c r="E4" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F4" t="s" s="10">
+      <c r="F4" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" ht="55.8" customHeight="1">
-      <c r="A5" t="s" s="10">
+    <row r="5" spans="1:6" ht="55.9" customHeight="1">
+      <c r="A5" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B5" t="s" s="11">
+      <c r="B5" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C5" t="s" s="10">
+      <c r="C5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D5" t="s" s="11">
+      <c r="D5" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E5" t="s" s="11">
+      <c r="E5" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F5" t="s" s="10">
+      <c r="F5" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" ht="55.8" customHeight="1">
-      <c r="A6" s="8"/>
-      <c r="B6" t="s" s="11">
+    <row r="6" spans="1:6" ht="55.9" customHeight="1">
+      <c r="A6" s="7"/>
+      <c r="B6" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C6" t="s" s="10">
+      <c r="C6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D6" t="s" s="11">
+      <c r="D6" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E6" t="s" s="11">
+      <c r="E6" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F6" t="s" s="10">
+      <c r="F6" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" ht="55.8" customHeight="1">
-      <c r="A7" s="8"/>
-      <c r="B7" t="s" s="11">
+    <row r="7" spans="1:6" ht="55.9" customHeight="1">
+      <c r="A7" s="7"/>
+      <c r="B7" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C7" t="s" s="10">
+      <c r="C7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D7" t="s" s="11">
+      <c r="D7" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E7" t="s" s="11">
+      <c r="E7" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F7" t="s" s="10">
+      <c r="F7" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" ht="55.8" customHeight="1">
-      <c r="A8" t="s" s="10">
+    <row r="8" spans="1:6" ht="55.9" customHeight="1">
+      <c r="A8" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B8" t="s" s="11">
+      <c r="B8" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C8" t="s" s="10">
+      <c r="C8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D8" t="s" s="11">
+      <c r="D8" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E8" t="s" s="11">
+      <c r="E8" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F8" t="s" s="10">
+      <c r="F8" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" ht="55.8" customHeight="1">
-      <c r="A9" s="8"/>
-      <c r="B9" t="s" s="11">
+    <row r="9" spans="1:6" ht="55.9" customHeight="1">
+      <c r="A9" s="7"/>
+      <c r="B9" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C9" t="s" s="10">
+      <c r="C9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D9" t="s" s="11">
+      <c r="D9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E9" t="s" s="11">
+      <c r="E9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F9" t="s" s="10">
+      <c r="F9" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" ht="55.8" customHeight="1">
-      <c r="A10" s="8"/>
-      <c r="B10" t="s" s="11">
+    <row r="10" spans="1:6" ht="55.9" customHeight="1">
+      <c r="A10" s="7"/>
+      <c r="B10" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C10" t="s" s="10">
+      <c r="C10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D10" t="s" s="11">
+      <c r="D10" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E10" t="s" s="11">
+      <c r="E10" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F10" t="s" s="10">
+      <c r="F10" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" ht="55.8" customHeight="1">
-      <c r="A11" s="8"/>
-      <c r="B11" t="s" s="11">
+    <row r="11" spans="1:6" ht="55.9" customHeight="1">
+      <c r="A11" s="7"/>
+      <c r="B11" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C11" t="s" s="10">
+      <c r="C11" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D11" t="s" s="11">
+      <c r="D11" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E11" t="s" s="11">
+      <c r="E11" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F11" t="s" s="10">
+      <c r="F11" s="9" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2388,15 +2496,15 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:C11">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal" stopIfTrue="1">
+    <cfRule type="cellIs" dxfId="5" priority="1" stopIfTrue="1" operator="equal">
       <formula>"failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal" stopIfTrue="1">
+    <cfRule type="cellIs" dxfId="4" priority="2" stopIfTrue="1" operator="equal">
       <formula>"passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -2404,177 +2512,211 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="69.6" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="69.599999999999994" customHeight="1"/>
   <cols>
-    <col min="1" max="6" width="14.5" style="15" customWidth="1"/>
-    <col min="7" max="16384" width="14.5" style="15" customWidth="1"/>
+    <col min="1" max="5" width="14.42578125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="14.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" ht="28.8" customHeight="1">
-      <c r="A1" t="s" s="10">
+    <row r="1" spans="1:6" ht="28.9" customHeight="1">
+      <c r="A1" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-    </row>
-    <row r="2" ht="25.8" customHeight="1">
-      <c r="A2" t="s" s="10">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+    </row>
+    <row r="2" spans="1:6" ht="25.9" customHeight="1">
+      <c r="A2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s" s="10">
+      <c r="B2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s" s="10">
+      <c r="C2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s" s="10">
+      <c r="D2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s" s="10">
+      <c r="E2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s" s="10">
+      <c r="F2" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" ht="123" customHeight="1">
-      <c r="A3" s="8"/>
-      <c r="B3" t="s" s="11">
+    <row r="3" spans="1:6" ht="123" customHeight="1">
+      <c r="A3" s="7"/>
+      <c r="B3" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C3" t="s" s="10">
+      <c r="C3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D3" t="s" s="11">
+      <c r="D3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E3" t="s" s="11">
+      <c r="E3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F3" t="s" s="10">
+      <c r="F3" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" ht="69.6" customHeight="1">
-      <c r="A4" t="s" s="10">
+    <row r="4" spans="1:6" ht="69.599999999999994" customHeight="1">
+      <c r="A4" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B4" t="s" s="11">
+      <c r="B4" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C4" t="s" s="10">
+      <c r="C4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D4" t="s" s="11">
+      <c r="D4" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="E4" t="s" s="11">
+      <c r="E4" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F4" t="s" s="10">
+      <c r="F4" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" ht="69.6" customHeight="1">
-      <c r="A5" s="8"/>
-      <c r="B5" t="s" s="11">
+    <row r="5" spans="1:6" ht="69.599999999999994" customHeight="1">
+      <c r="A5" s="7"/>
+      <c r="B5" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C5" t="s" s="10">
+      <c r="C5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D5" t="s" s="11">
+      <c r="D5" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="E5" t="s" s="11">
+      <c r="E5" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="F5" t="s" s="10">
+      <c r="F5" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" ht="69.6" customHeight="1">
-      <c r="A6" s="8"/>
-      <c r="B6" t="s" s="11">
+    <row r="6" spans="1:6" ht="69.599999999999994" customHeight="1">
+      <c r="A6" s="7"/>
+      <c r="B6" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C6" t="s" s="10">
+      <c r="C6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D6" t="s" s="11">
+      <c r="D6" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E6" t="s" s="11">
+      <c r="E6" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F6" t="s" s="10">
+      <c r="F6" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" ht="69.6" customHeight="1">
-      <c r="A7" s="8"/>
-      <c r="B7" t="s" s="11">
+    <row r="7" spans="1:6" ht="69.599999999999994" customHeight="1">
+      <c r="A7" s="7"/>
+      <c r="B7" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C7" t="s" s="10">
+      <c r="C7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D7" t="s" s="11">
+      <c r="D7" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E7" t="s" s="11">
+      <c r="E7" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F7" t="s" s="10">
+      <c r="F7" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-    </row>
-    <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-    </row>
-    <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
+    <row r="8" spans="1:6" ht="129.75" customHeight="1">
+      <c r="A8" s="32"/>
+      <c r="B8" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="112.5" customHeight="1">
+      <c r="A9" s="32"/>
+      <c r="B9" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" s="32" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="102" customHeight="1">
+      <c r="A10" s="32"/>
+      <c r="B10" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>49</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:C7">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal" stopIfTrue="1">
+    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="equal">
       <formula>"failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal" stopIfTrue="1">
+    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="equal">
       <formula>"passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -2582,175 +2724,178 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:F1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.5" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.6328" style="16" customWidth="1"/>
-    <col min="3" max="3" width="47.4062" style="16" customWidth="1"/>
-    <col min="4" max="4" width="14.5" style="16" customWidth="1"/>
-    <col min="5" max="5" width="28.4219" style="16" customWidth="1"/>
-    <col min="6" max="6" width="29.4375" style="16" customWidth="1"/>
-    <col min="7" max="16384" width="8.85156" style="16" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="47.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="28.42578125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="29.42578125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="17">
+    <row r="1" spans="1:6" ht="13.5" customHeight="1">
+      <c r="A1" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-    </row>
-    <row r="2" ht="144" customHeight="1">
-      <c r="A2" t="s" s="19">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+    </row>
+    <row r="2" spans="1:6" ht="144" customHeight="1">
+      <c r="A2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-    </row>
-    <row r="3" ht="57.6" customHeight="1">
-      <c r="A3" t="s" s="21">
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+    </row>
+    <row r="3" spans="1:6" ht="57.6" customHeight="1">
+      <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s" s="22">
+      <c r="B3" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C3" t="s" s="23">
+      <c r="C3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s" s="23">
+      <c r="D3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s" s="23">
+      <c r="E3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F3" t="s" s="23">
+      <c r="F3" s="16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" ht="86.4" customHeight="1">
-      <c r="A4" t="s" s="24">
+    <row r="4" spans="1:6" ht="86.45" customHeight="1">
+      <c r="A4" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="25">
+      <c r="B4" s="18">
         <v>1</v>
       </c>
-      <c r="C4" t="s" s="26">
+      <c r="C4" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="D4" t="s" s="27">
+      <c r="D4" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E4" t="s" s="26">
+      <c r="E4" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="F4" t="s" s="26">
+      <c r="F4" s="19" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" ht="26.55" customHeight="1">
-      <c r="A5" t="s" s="24">
+    <row r="5" spans="1:6" ht="26.65" customHeight="1">
+      <c r="A5" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="25">
+      <c r="B5" s="18">
         <v>1</v>
       </c>
-      <c r="C5" t="s" s="28">
+      <c r="C5" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="D5" t="s" s="27">
+      <c r="D5" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E5" t="s" s="28">
+      <c r="E5" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="F5" t="s" s="28">
+      <c r="F5" s="21" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="6" ht="26.55" customHeight="1">
-      <c r="A6" s="29"/>
-      <c r="B6" s="25">
+    <row r="6" spans="1:6" ht="26.65" customHeight="1">
+      <c r="A6" s="22"/>
+      <c r="B6" s="18">
         <v>2</v>
       </c>
-      <c r="C6" t="s" s="28">
+      <c r="C6" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="D6" t="s" s="27">
+      <c r="D6" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E6" t="s" s="28">
+      <c r="E6" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="F6" t="s" s="28">
+      <c r="F6" s="21" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="7" ht="26.55" customHeight="1">
-      <c r="A7" t="s" s="24">
+    <row r="7" spans="1:6" ht="26.65" customHeight="1">
+      <c r="A7" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="25">
+      <c r="B7" s="18">
         <v>1</v>
       </c>
-      <c r="C7" t="s" s="28">
+      <c r="C7" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="D7" t="s" s="27">
+      <c r="D7" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E7" t="s" s="28">
+      <c r="E7" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="F7" t="s" s="28">
+      <c r="F7" s="21" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="8" ht="14.7" customHeight="1">
-      <c r="A8" s="29"/>
-      <c r="B8" s="25">
+    <row r="8" spans="1:6" ht="14.65" customHeight="1">
+      <c r="A8" s="22"/>
+      <c r="B8" s="18">
         <v>2</v>
       </c>
-      <c r="C8" t="s" s="28">
+      <c r="C8" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="D8" t="s" s="27">
+      <c r="D8" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E8" t="s" s="28">
+      <c r="E8" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="F8" t="s" s="28">
+      <c r="F8" s="21" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="9" ht="26.7" customHeight="1">
-      <c r="A9" t="s" s="24">
+    <row r="9" spans="1:6" ht="26.65" customHeight="1">
+      <c r="A9" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="25">
+      <c r="B9" s="18">
         <v>1</v>
       </c>
-      <c r="C9" t="s" s="28">
+      <c r="C9" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="D9" t="s" s="27">
+      <c r="D9" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E9" t="s" s="28">
+      <c r="E9" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="F9" t="s" s="28">
+      <c r="F9" s="21" t="s">
         <v>71</v>
       </c>
     </row>
@@ -2759,15 +2904,15 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D9">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal" stopIfTrue="1">
+    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="equal">
       <formula>"failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal" stopIfTrue="1">
+    <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="equal">
       <formula>"passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Add test cases for authentication in test_log.xlsx
</commit_message>
<xml_diff>
--- a/test_log.xlsx
+++ b/test_log.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karan\Documents\GitHub\SzoftverfejlesztesModszertanMiniProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\nandi\szoftvermodszertan\SzoftverfejlesztesModszertanMiniProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE9469EF-6B91-4938-8252-169392434C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="122">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -256,12 +255,147 @@
   </si>
   <si>
     <t>Number of dislikes are increased</t>
+  </si>
+  <si>
+    <t>User submits login form with valid credentials</t>
+  </si>
+  <si>
+    <t>User enters valid email and password and submits the login form</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>User is redirected to the main page, and the token is stored in local storage</t>
+  </si>
+  <si>
+    <t>User submits login form with invalid email</t>
+  </si>
+  <si>
+    <t>User enters an invalid email format and submits the login form</t>
+  </si>
+  <si>
+    <t>Error message: "Invalid email format" is displayed</t>
+  </si>
+  <si>
+    <t>User submits login form with incorrect credentials</t>
+  </si>
+  <si>
+    <t>User enters valid email but incorrect password and submits the form</t>
+  </si>
+  <si>
+    <t>Error message: "Invalid email or password" is displayed</t>
+  </si>
+  <si>
+    <t>User attempts login without entering email</t>
+  </si>
+  <si>
+    <t>User submits the login form with an empty email field</t>
+  </si>
+  <si>
+    <t>Error message: "Please fill in both fields" is displayed</t>
+  </si>
+  <si>
+    <t>User attempts login without entering password</t>
+  </si>
+  <si>
+    <t>User submits the login form with an empty password field</t>
+  </si>
+  <si>
+    <t>User clicks on "Forgot Password" link</t>
+  </si>
+  <si>
+    <t>User clicks the "Forgot Password" link</t>
+  </si>
+  <si>
+    <t>User is redirected to the password reset page</t>
+  </si>
+  <si>
+    <t>User logs out successfully</t>
+  </si>
+  <si>
+    <t>User clicks the logout button</t>
+  </si>
+  <si>
+    <t>User is redirected to the login page, and the token is cleared from local storage</t>
+  </si>
+  <si>
+    <t>POST /auth/signin with valid credentials</t>
+  </si>
+  <si>
+    <t>Send a post request to the backend with a valid email and password</t>
+  </si>
+  <si>
+    <t>The server responds with status code 200 and user data</t>
+  </si>
+  <si>
+    <t>POST /auth/signin with incorrect email</t>
+  </si>
+  <si>
+    <t>Send a post request to the backend with an invalid email format</t>
+  </si>
+  <si>
+    <t>The server responds with error code 400 (Bad Request)</t>
+  </si>
+  <si>
+    <t>POST /auth/signin with incorrect password</t>
+  </si>
+  <si>
+    <t>Send a post request to the backend with a valid email but incorrect password</t>
+  </si>
+  <si>
+    <t>The server responds with error code 401 (Unauthorized)</t>
+  </si>
+  <si>
+    <t>POST /auth/signup with already existing email</t>
+  </si>
+  <si>
+    <t>Send a post request to the backend with a previously used email address</t>
+  </si>
+  <si>
+    <t>The server responds with error code 409 (Conflict)</t>
+  </si>
+  <si>
+    <t>POST /auth/signup with valid credentials</t>
+  </si>
+  <si>
+    <t>Send a post request to the backend with valid username, email, and password</t>
+  </si>
+  <si>
+    <t>The server responds with status code 201 (Created) and user data</t>
+  </si>
+  <si>
+    <t>POST /auth/signup with missing required fields</t>
+  </si>
+  <si>
+    <t>Send a post request to the backend with missing username, email, or password</t>
+  </si>
+  <si>
+    <t>GET /auth/me with valid token</t>
+  </si>
+  <si>
+    <t>Send a GET request to the backend with a valid JWT token</t>
+  </si>
+  <si>
+    <t>The server responds with status code 200 and the authenticated user data</t>
+  </si>
+  <si>
+    <t>GET /auth/me with invalid token</t>
+  </si>
+  <si>
+    <t>Send a GET request to the backend with an invalid JWT token</t>
+  </si>
+  <si>
+    <t>POST /auth/refresh-token with expired token</t>
+  </si>
+  <si>
+    <t>Send a post request to the backend with an expired refresh token</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -501,7 +635,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -565,6 +699,18 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -587,21 +733,31 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - 6. jelölőszín" xfId="1" builtinId="52"/>
+    <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="14"/>
+          <bgColor indexed="16"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="14"/>
+          <bgColor indexed="15"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1807,7 +1963,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D18"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -1821,11 +1977,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="0" hidden="1" customHeight="1">
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
     </row>
     <row r="7" spans="2:4" ht="18.75">
       <c r="B7" s="1" t="s">
@@ -1923,18 +2079,18 @@
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D10" location="'test_DB'!R1C1" display="test_DB" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D12" location="'test_MB'!R1C1" display="test_MB" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D14" location="'test_VN'!R1C1" display="test_VN" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="D16" location="'test_KM'!R1C1" display="test_KM" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="D18" location="'test_SZ'!R1C1" display="test_SZ" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D10" location="'test_DB'!R1C1" display="test_DB"/>
+    <hyperlink ref="D12" location="'test_MB'!R1C1" display="test_MB"/>
+    <hyperlink ref="D14" location="'test_VN'!R1C1" display="test_VN"/>
+    <hyperlink ref="D16" location="'test_KM'!R1C1" display="test_KM"/>
+    <hyperlink ref="D18" location="'test_SZ'!R1C1" display="test_SZ"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -1952,14 +2108,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="13.5" customHeight="1">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="27"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="31"/>
     </row>
     <row r="2" spans="1:6" ht="13.5" customHeight="1">
       <c r="A2" s="6" t="s">
@@ -2094,10 +2250,10 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:C6 D9:D10">
-    <cfRule type="cellIs" dxfId="9" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" stopIfTrue="1" operator="equal">
       <formula>"failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" stopIfTrue="1" operator="equal">
       <formula>"passed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2110,7 +2266,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -2128,15 +2284,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
     </row>
     <row r="2" spans="1:7" ht="13.5" customHeight="1">
       <c r="A2" s="9" t="s">
@@ -2268,6 +2424,234 @@
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:C5">
+    <cfRule type="cellIs" dxfId="9" priority="1" stopIfTrue="1" operator="equal">
+      <formula>"failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"passed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="55.9" customHeight="1"/>
+  <cols>
+    <col min="1" max="7" width="15.140625" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="15.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="55.9" customHeight="1">
+      <c r="A1" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+    </row>
+    <row r="2" spans="1:6" ht="55.9" customHeight="1">
+      <c r="A2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="55.9" customHeight="1">
+      <c r="A3" s="7"/>
+      <c r="B3" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="55.9" customHeight="1">
+      <c r="A4" s="7"/>
+      <c r="B4" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="55.9" customHeight="1">
+      <c r="A5" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="55.9" customHeight="1">
+      <c r="A6" s="7"/>
+      <c r="B6" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="55.9" customHeight="1">
+      <c r="A7" s="7"/>
+      <c r="B7" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="55.9" customHeight="1">
+      <c r="A8" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="55.9" customHeight="1">
+      <c r="A9" s="7"/>
+      <c r="B9" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="55.9" customHeight="1">
+      <c r="A10" s="7"/>
+      <c r="B10" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="55.9" customHeight="1">
+      <c r="A11" s="7"/>
+      <c r="B11" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C2:C11">
     <cfRule type="cellIs" dxfId="7" priority="1" stopIfTrue="1" operator="equal">
       <formula>"failed"</formula>
     </cfRule>
@@ -2283,259 +2667,34 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F11"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="55.9" customHeight="1"/>
-  <cols>
-    <col min="1" max="7" width="15.140625" style="5" customWidth="1"/>
-    <col min="8" max="16384" width="15.140625" style="5"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="55.9" customHeight="1">
-      <c r="A1" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-    </row>
-    <row r="2" spans="1:6" ht="55.9" customHeight="1">
-      <c r="A2" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="55.9" customHeight="1">
-      <c r="A3" s="7"/>
-      <c r="B3" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="55.9" customHeight="1">
-      <c r="A4" s="7"/>
-      <c r="B4" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="55.9" customHeight="1">
-      <c r="A5" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="55.9" customHeight="1">
-      <c r="A6" s="7"/>
-      <c r="B6" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="55.9" customHeight="1">
-      <c r="A7" s="7"/>
-      <c r="B7" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="55.9" customHeight="1">
-      <c r="A8" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="55.9" customHeight="1">
-      <c r="A9" s="7"/>
-      <c r="B9" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="55.9" customHeight="1">
-      <c r="A10" s="7"/>
-      <c r="B10" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="55.9" customHeight="1">
-      <c r="A11" s="7"/>
-      <c r="B11" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
-  </mergeCells>
-  <conditionalFormatting sqref="C2:C11">
-    <cfRule type="cellIs" dxfId="5" priority="1" stopIfTrue="1" operator="equal">
-      <formula>"failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" stopIfTrue="1" operator="equal">
-      <formula>"passed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:F10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="69.599999999999994" customHeight="1"/>
   <cols>
-    <col min="1" max="5" width="14.42578125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="20.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" style="5" customWidth="1"/>
     <col min="7" max="7" width="14.42578125" style="5" customWidth="1"/>
     <col min="8" max="16384" width="14.42578125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="28.9" customHeight="1">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
     </row>
     <row r="2" spans="1:6" ht="25.9" customHeight="1">
       <c r="A2" s="9" t="s">
@@ -2650,57 +2809,377 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="129.75" customHeight="1">
-      <c r="A8" s="32"/>
-      <c r="B8" s="32" t="s">
+      <c r="A8" s="25"/>
+      <c r="B8" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="32" t="s">
+      <c r="E8" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="32" t="s">
+      <c r="F8" s="25" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="112.5" customHeight="1">
-      <c r="A9" s="32"/>
-      <c r="B9" s="32" t="s">
+      <c r="A9" s="25"/>
+      <c r="B9" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="32" t="s">
+      <c r="D9" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="E9" s="32" t="s">
+      <c r="E9" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="F9" s="32" t="s">
+      <c r="F9" s="25" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="102" customHeight="1">
-      <c r="A10" s="32"/>
-      <c r="B10" s="32" t="s">
+      <c r="A10" s="25"/>
+      <c r="B10" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="C10" s="33" t="s">
+      <c r="C10" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="32" t="s">
+      <c r="D10" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="E10" s="32" t="s">
+      <c r="E10" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="F10" s="32" t="s">
+      <c r="F10" s="25" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="69.599999999999994" customHeight="1">
+      <c r="A11" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="69.599999999999994" customHeight="1">
+      <c r="A12" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="69.599999999999994" customHeight="1">
+      <c r="A13" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="69.599999999999994" customHeight="1">
+      <c r="A14" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="69.599999999999994" customHeight="1">
+      <c r="A15" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="69.599999999999994" customHeight="1">
+      <c r="A16" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="69.599999999999994" customHeight="1">
+      <c r="A17" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="69.599999999999994" customHeight="1">
+      <c r="A18" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="69.599999999999994" customHeight="1">
+      <c r="A19" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="69.599999999999994" customHeight="1">
+      <c r="A20" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="69.599999999999994" customHeight="1">
+      <c r="A21" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="69.599999999999994" customHeight="1">
+      <c r="A22" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="69.599999999999994" customHeight="1">
+      <c r="A23" s="35" t="s">
+        <v>113</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="69.599999999999994" customHeight="1">
+      <c r="A24" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="E24" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="69.599999999999994" customHeight="1">
+      <c r="A25" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="69.599999999999994" customHeight="1">
+      <c r="A26" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2708,10 +3187,18 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:C7">
-    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" stopIfTrue="1" operator="equal">
       <formula>"failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"passed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:C16 C18:C23 C25:C26">
+    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="equal">
+      <formula>"failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="equal">
       <formula>"passed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2724,7 +3211,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2744,14 +3231,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="13.5" customHeight="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
     </row>
     <row r="2" spans="1:6" ht="144" customHeight="1">
       <c r="A2" s="12" t="s">
@@ -2904,10 +3391,10 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D9">
-    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="equal">
       <formula>"failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="equal">
       <formula>"passed"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
feat: Adding test reports: Monár Bálint
</commit_message>
<xml_diff>
--- a/test_log.xlsx
+++ b/test_log.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\nandi\szoftvermodszertan\SzoftverfejlesztesModszertanMiniProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\molnar.balint\Desktop\Egyetem\Szoftmod\SzoftverfejlesztesModszertanMiniProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F448EDE6-F534-4A08-89F2-39BD10018D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="150">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -390,12 +391,96 @@
   </si>
   <si>
     <t>Send a post request to the backend with an expired refresh token</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Case </t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Actual Result</t>
+  </si>
+  <si>
+    <t>Create blog post</t>
+  </si>
+  <si>
+    <t>Update blog post</t>
+  </si>
+  <si>
+    <t>Delete blog post</t>
+  </si>
+  <si>
+    <t>Get blog posts</t>
+  </si>
+  <si>
+    <t>Translate blog post</t>
+  </si>
+  <si>
+    <t>Get activities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hide activity </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check activity </t>
+  </si>
+  <si>
+    <t>Create blog post by the given data</t>
+  </si>
+  <si>
+    <t>Update blog post by the given data</t>
+  </si>
+  <si>
+    <t>Successfully create new post and navigate back to own posts</t>
+  </si>
+  <si>
+    <t>Succesful update and refresh</t>
+  </si>
+  <si>
+    <t>Successful delete and blog post disappear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Molnár Bálint </t>
+  </si>
+  <si>
+    <t>Blog posts successfully rendered into a list</t>
+  </si>
+  <si>
+    <t>Translate blog post to HU</t>
+  </si>
+  <si>
+    <t>Successful translation to HU</t>
+  </si>
+  <si>
+    <t>Get all activities and listing them</t>
+  </si>
+  <si>
+    <t>Sucessful activity listing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hide the selected activity </t>
+  </si>
+  <si>
+    <t>Successful hide operation, UI refresh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you created a blog post you can check it through an activity </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Succesful activity check, you can navigate to blog post </t>
+  </si>
+  <si>
+    <t>Validated by: Molnár Bálint</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -437,7 +522,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -486,8 +571,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -630,12 +727,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -699,9 +811,6 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -709,6 +818,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -733,9 +845,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="60% - 6. jelölőszín" xfId="1" builtinId="52"/>
@@ -1963,7 +2078,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:D18"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2079,18 +2194,18 @@
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D10" location="'test_DB'!R1C1" display="test_DB"/>
-    <hyperlink ref="D12" location="'test_MB'!R1C1" display="test_MB"/>
-    <hyperlink ref="D14" location="'test_VN'!R1C1" display="test_VN"/>
-    <hyperlink ref="D16" location="'test_KM'!R1C1" display="test_KM"/>
-    <hyperlink ref="D18" location="'test_SZ'!R1C1" display="test_SZ"/>
+    <hyperlink ref="D10" location="'test_DB'!R1C1" display="test_DB" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D12" location="'test_MB'!R1C1" display="test_MB" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D14" location="'test_VN'!R1C1" display="test_VN" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D16" location="'test_KM'!R1C1" display="test_KM" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D18" location="'test_SZ'!R1C1" display="test_SZ" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -2266,20 +2381,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="9" style="5" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="5" customWidth="1"/>
-    <col min="7" max="8" width="8.85546875" style="5" customWidth="1"/>
+    <col min="1" max="1" width="38" style="5" customWidth="1"/>
+    <col min="2" max="2" width="40.5703125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="36.42578125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="5" customWidth="1"/>
     <col min="9" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
@@ -2313,7 +2431,9 @@
       <c r="F2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="11"/>
+      <c r="G2" s="11" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="45" customHeight="1">
       <c r="A3" s="9" t="s">
@@ -2334,7 +2454,9 @@
       <c r="F3" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="11"/>
+      <c r="G3" s="35">
+        <v>45608</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="54" customHeight="1">
       <c r="A4" s="7"/>
@@ -2353,7 +2475,9 @@
       <c r="F4" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="11"/>
+      <c r="G4" s="35">
+        <v>45608</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="47.45" customHeight="1">
       <c r="A5" s="7"/>
@@ -2372,7 +2496,9 @@
       <c r="F5" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="11"/>
+      <c r="G5" s="35">
+        <v>45608</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="13.5" customHeight="1">
       <c r="A6" s="11"/>
@@ -2418,6 +2544,218 @@
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
+    </row>
+    <row r="14" spans="1:7" ht="14.45" customHeight="1">
+      <c r="A14" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="B14" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="C14" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="39" t="s">
+        <v>125</v>
+      </c>
+      <c r="F14" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="39" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="14.45" customHeight="1">
+      <c r="A15" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="B15" s="36" t="s">
+        <v>134</v>
+      </c>
+      <c r="C15" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="36" t="s">
+        <v>136</v>
+      </c>
+      <c r="E15" s="36" t="s">
+        <v>136</v>
+      </c>
+      <c r="F15" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" s="38">
+        <v>45634</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="14.45" customHeight="1">
+      <c r="A16" s="36" t="s">
+        <v>127</v>
+      </c>
+      <c r="B16" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="C16" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="E16" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="F16" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" s="38">
+        <v>45634</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="14.45" customHeight="1">
+      <c r="A17" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="B17" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="C17" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="36" t="s">
+        <v>138</v>
+      </c>
+      <c r="E17" s="36" t="s">
+        <v>138</v>
+      </c>
+      <c r="F17" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="G17" s="38">
+        <v>45634</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="14.45" customHeight="1">
+      <c r="A18" s="36" t="s">
+        <v>129</v>
+      </c>
+      <c r="B18" s="36" t="s">
+        <v>129</v>
+      </c>
+      <c r="C18" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="E18" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="F18" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="G18" s="38">
+        <v>45634</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="14.45" customHeight="1">
+      <c r="A19" s="36" t="s">
+        <v>130</v>
+      </c>
+      <c r="B19" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="C19" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="E19" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="F19" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="G19" s="38">
+        <v>45634</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="14.45" customHeight="1">
+      <c r="A20" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="B20" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="C20" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="E20" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="F20" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="G20" s="38">
+        <v>45634</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="14.45" customHeight="1">
+      <c r="A21" s="36" t="s">
+        <v>132</v>
+      </c>
+      <c r="B21" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="C21" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="36" t="s">
+        <v>146</v>
+      </c>
+      <c r="E21" s="36" t="s">
+        <v>146</v>
+      </c>
+      <c r="F21" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="G21" s="38">
+        <v>45634</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="14.45" customHeight="1">
+      <c r="A22" s="36" t="s">
+        <v>133</v>
+      </c>
+      <c r="B22" s="36" t="s">
+        <v>147</v>
+      </c>
+      <c r="C22" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="36" t="s">
+        <v>148</v>
+      </c>
+      <c r="E22" s="36" t="s">
+        <v>148</v>
+      </c>
+      <c r="F22" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="G22" s="38">
+        <v>45634</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="14.45" customHeight="1">
+      <c r="A23" s="40" t="s">
+        <v>149</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2440,7 +2778,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -2668,10 +3006,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
@@ -2809,56 +3147,56 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="129.75" customHeight="1">
-      <c r="A8" s="25"/>
-      <c r="B8" s="25" t="s">
+      <c r="A8" s="24"/>
+      <c r="B8" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="F8" s="24" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="112.5" customHeight="1">
-      <c r="A9" s="25"/>
-      <c r="B9" s="25" t="s">
+      <c r="A9" s="24"/>
+      <c r="B9" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="24" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="102" customHeight="1">
-      <c r="A10" s="25"/>
-      <c r="B10" s="25" t="s">
+      <c r="A10" s="24"/>
+      <c r="B10" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="F10" s="25" t="s">
+      <c r="F10" s="24" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2878,12 +3216,12 @@
       <c r="E11" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="F11" s="23" t="s">
+      <c r="F11" s="9" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="69.599999999999994" customHeight="1">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="26" t="s">
         <v>81</v>
       </c>
       <c r="B12" s="10" t="s">
@@ -2898,7 +3236,7 @@
       <c r="E12" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="F12" s="23" t="s">
+      <c r="F12" s="9" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2918,12 +3256,12 @@
       <c r="E13" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F13" s="23" t="s">
+      <c r="F13" s="9" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="69.599999999999994" customHeight="1">
-      <c r="A14" s="35" t="s">
+      <c r="A14" s="26" t="s">
         <v>87</v>
       </c>
       <c r="B14" s="10" t="s">
@@ -2938,12 +3276,12 @@
       <c r="E14" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="F14" s="23" t="s">
+      <c r="F14" s="9" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="69.599999999999994" customHeight="1">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="26" t="s">
         <v>90</v>
       </c>
       <c r="B15" s="10" t="s">
@@ -2958,12 +3296,12 @@
       <c r="E15" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="F15" s="23" t="s">
+      <c r="F15" s="9" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="69.599999999999994" customHeight="1">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="26" t="s">
         <v>92</v>
       </c>
       <c r="B16" s="10" t="s">
@@ -2978,27 +3316,27 @@
       <c r="E16" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="F16" s="23" t="s">
+      <c r="F16" s="9" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="69.599999999999994" customHeight="1">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="D17" s="25" t="s">
+      <c r="D17" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="E17" s="25" t="s">
+      <c r="E17" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="F17" s="23" t="s">
+      <c r="F17" s="9" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3018,12 +3356,12 @@
       <c r="E18" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="F18" s="23" t="s">
+      <c r="F18" s="9" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="69.599999999999994" customHeight="1">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="26" t="s">
         <v>101</v>
       </c>
       <c r="B19" s="10" t="s">
@@ -3038,7 +3376,7 @@
       <c r="E19" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="F19" s="23" t="s">
+      <c r="F19" s="9" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3058,12 +3396,12 @@
       <c r="E20" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="F20" s="23" t="s">
+      <c r="F20" s="9" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="69.599999999999994" customHeight="1">
-      <c r="A21" s="35" t="s">
+      <c r="A21" s="26" t="s">
         <v>107</v>
       </c>
       <c r="B21" s="10" t="s">
@@ -3078,12 +3416,12 @@
       <c r="E21" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="F21" s="23" t="s">
+      <c r="F21" s="9" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="69.599999999999994" customHeight="1">
-      <c r="A22" s="35" t="s">
+      <c r="A22" s="26" t="s">
         <v>110</v>
       </c>
       <c r="B22" s="10" t="s">
@@ -3098,12 +3436,12 @@
       <c r="E22" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="F22" s="23" t="s">
+      <c r="F22" s="9" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="69.599999999999994" customHeight="1">
-      <c r="A23" s="35" t="s">
+      <c r="A23" s="26" t="s">
         <v>113</v>
       </c>
       <c r="B23" s="10" t="s">
@@ -3118,27 +3456,27 @@
       <c r="E23" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="F23" s="23" t="s">
+      <c r="F23" s="9" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="69.599999999999994" customHeight="1">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="B24" s="25" t="s">
+      <c r="B24" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="C24" s="24" t="s">
+      <c r="C24" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="D24" s="25" t="s">
+      <c r="D24" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="E24" s="25" t="s">
+      <c r="E24" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="F24" s="23" t="s">
+      <c r="F24" s="9" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3158,12 +3496,12 @@
       <c r="E25" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="F25" s="23" t="s">
+      <c r="F25" s="9" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="69.599999999999994" customHeight="1">
-      <c r="A26" s="35" t="s">
+      <c r="A26" s="26" t="s">
         <v>120</v>
       </c>
       <c r="B26" s="10" t="s">
@@ -3178,7 +3516,7 @@
       <c r="E26" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="F26" s="23" t="s">
+      <c r="F26" s="9" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3195,10 +3533,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:C16 C18:C23 C25:C26">
-    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="equal">
       <formula>"failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="equal">
       <formula>"passed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3211,7 +3549,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3391,10 +3729,10 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D9">
-    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="equal">
       <formula>"failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="equal">
       <formula>"passed"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
test: Testing login, registration and Accounts page and reported the test results into test_log.xlsx
</commit_message>
<xml_diff>
--- a/test_log.xlsx
+++ b/test_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\molnar.balint\Desktop\Egyetem\Szoftmod\SzoftverfejlesztesModszertanMiniProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F448EDE6-F534-4A08-89F2-39BD10018D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266DA9C0-1498-4A58-B073-14F1DE00A484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="161">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -475,13 +475,46 @@
   </si>
   <si>
     <t>Validated by: Molnár Bálint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login </t>
+  </si>
+  <si>
+    <t>Registration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accounts </t>
+  </si>
+  <si>
+    <t>Listing existing accounts in the system</t>
+  </si>
+  <si>
+    <t>Successful account listing</t>
+  </si>
+  <si>
+    <t>Register a new user with username, email, password</t>
+  </si>
+  <si>
+    <t>Successfull registration</t>
+  </si>
+  <si>
+    <t>Drevenyák Bálint, Vardbíró Nándor</t>
+  </si>
+  <si>
+    <t>Karancsi Mátyás, Vardbíró Nándor</t>
+  </si>
+  <si>
+    <t>Succesful login and redirect to own posts</t>
+  </si>
+  <si>
+    <t>Login with username and password</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -521,8 +554,15 @@
       <color indexed="21"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -580,6 +620,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -747,7 +799,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -823,6 +875,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -845,12 +902,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="60% - 6. jelölőszín" xfId="1" builtinId="52"/>
@@ -2092,11 +2150,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="0" hidden="1" customHeight="1">
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
     </row>
     <row r="7" spans="2:4" ht="18.75">
       <c r="B7" s="1" t="s">
@@ -2223,14 +2281,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="13.5" customHeight="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="31"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="36"/>
     </row>
     <row r="2" spans="1:6" ht="13.5" customHeight="1">
       <c r="A2" s="6" t="s">
@@ -2382,10 +2440,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45" customHeight="1"/>
@@ -2402,36 +2460,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
     </row>
     <row r="2" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="43" t="s">
         <v>122</v>
       </c>
     </row>
@@ -2454,7 +2512,7 @@
       <c r="F3" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="35">
+      <c r="G3" s="27">
         <v>45608</v>
       </c>
     </row>
@@ -2475,7 +2533,7 @@
       <c r="F4" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="35">
+      <c r="G4" s="27">
         <v>45608</v>
       </c>
     </row>
@@ -2496,7 +2554,7 @@
       <c r="F5" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="35">
+      <c r="G5" s="27">
         <v>45608</v>
       </c>
     </row>
@@ -2546,214 +2604,283 @@
       <c r="G10" s="11"/>
     </row>
     <row r="14" spans="1:7" ht="14.45" customHeight="1">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="C14" s="39" t="s">
+      <c r="C14" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="39" t="s">
+      <c r="D14" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="39" t="s">
+      <c r="E14" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="F14" s="39" t="s">
+      <c r="F14" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="39" t="s">
+      <c r="G14" s="31" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="14.45" customHeight="1">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="36" t="s">
+      <c r="D15" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="E15" s="36" t="s">
+      <c r="E15" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="F15" s="36" t="s">
+      <c r="F15" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="38">
+      <c r="G15" s="30">
         <v>45634</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="14.45" customHeight="1">
-      <c r="A16" s="36" t="s">
+      <c r="A16" s="28" t="s">
         <v>127</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="C16" s="37" t="s">
+      <c r="C16" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="36" t="s">
+      <c r="D16" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="E16" s="36" t="s">
+      <c r="E16" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="F16" s="36" t="s">
+      <c r="F16" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="G16" s="38">
+      <c r="G16" s="30">
         <v>45634</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="14.45" customHeight="1">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="C17" s="37" t="s">
+      <c r="C17" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="36" t="s">
+      <c r="D17" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="E17" s="36" t="s">
+      <c r="E17" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="F17" s="36" t="s">
+      <c r="F17" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="G17" s="38">
+      <c r="G17" s="30">
         <v>45634</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="14.45" customHeight="1">
-      <c r="A18" s="36" t="s">
+      <c r="A18" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="C18" s="37" t="s">
+      <c r="C18" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="36" t="s">
+      <c r="D18" s="28" t="s">
         <v>140</v>
       </c>
-      <c r="E18" s="36" t="s">
+      <c r="E18" s="28" t="s">
         <v>140</v>
       </c>
-      <c r="F18" s="36" t="s">
+      <c r="F18" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="G18" s="38">
+      <c r="G18" s="30">
         <v>45634</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="14.45" customHeight="1">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="C19" s="37" t="s">
+      <c r="C19" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="36" t="s">
+      <c r="D19" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="E19" s="36" t="s">
+      <c r="E19" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="F19" s="36" t="s">
+      <c r="F19" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="G19" s="38">
+      <c r="G19" s="30">
         <v>45634</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="14.45" customHeight="1">
-      <c r="A20" s="36" t="s">
+      <c r="A20" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="C20" s="37" t="s">
+      <c r="C20" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="36" t="s">
+      <c r="D20" s="28" t="s">
         <v>144</v>
       </c>
-      <c r="E20" s="36" t="s">
+      <c r="E20" s="28" t="s">
         <v>144</v>
       </c>
-      <c r="F20" s="36" t="s">
+      <c r="F20" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="G20" s="38">
+      <c r="G20" s="30">
         <v>45634</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="14.45" customHeight="1">
-      <c r="A21" s="36" t="s">
+      <c r="A21" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="C21" s="37" t="s">
+      <c r="C21" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="36" t="s">
+      <c r="D21" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="E21" s="36" t="s">
+      <c r="E21" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="F21" s="36" t="s">
+      <c r="F21" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="G21" s="38">
+      <c r="G21" s="30">
         <v>45634</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="14.45" customHeight="1">
-      <c r="A22" s="36" t="s">
+      <c r="A22" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="C22" s="37" t="s">
+      <c r="C22" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="36" t="s">
+      <c r="D22" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="E22" s="36" t="s">
+      <c r="E22" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="F22" s="36" t="s">
+      <c r="F22" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="G22" s="38">
+      <c r="G22" s="30">
         <v>45634</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="14.45" customHeight="1">
       <c r="A23" s="40" t="s">
+        <v>150</v>
+      </c>
+      <c r="B23" s="41" t="s">
+        <v>160</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="41" t="s">
+        <v>159</v>
+      </c>
+      <c r="E23" s="41" t="s">
+        <v>159</v>
+      </c>
+      <c r="F23" s="41" t="s">
+        <v>158</v>
+      </c>
+      <c r="G23" s="30">
+        <v>45635</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="14.45" customHeight="1">
+      <c r="A24" s="41" t="s">
+        <v>151</v>
+      </c>
+      <c r="B24" s="41" t="s">
+        <v>155</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="41" t="s">
+        <v>156</v>
+      </c>
+      <c r="E24" s="41" t="s">
+        <v>156</v>
+      </c>
+      <c r="F24" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="G24" s="30">
+        <v>45635</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="14.45" customHeight="1">
+      <c r="A25" s="41" t="s">
+        <v>152</v>
+      </c>
+      <c r="B25" s="41" t="s">
+        <v>153</v>
+      </c>
+      <c r="C25" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="41" t="s">
+        <v>154</v>
+      </c>
+      <c r="E25" s="41" t="s">
+        <v>154</v>
+      </c>
+      <c r="F25" s="41" t="s">
+        <v>139</v>
+      </c>
+      <c r="G25" s="30">
+        <v>45635</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="14.45" customHeight="1">
+      <c r="A26" s="44" t="s">
         <v>149</v>
       </c>
     </row>
@@ -2790,14 +2917,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="55.9" customHeight="1">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
     </row>
     <row r="2" spans="1:6" ht="55.9" customHeight="1">
       <c r="A2" s="9" t="s">
@@ -3025,14 +3152,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="28.9" customHeight="1">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
     </row>
     <row r="2" spans="1:6" ht="25.9" customHeight="1">
       <c r="A2" s="9" t="s">
@@ -3569,14 +3696,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="13.5" customHeight="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
     </row>
     <row r="2" spans="1:6" ht="144" customHeight="1">
       <c r="A2" s="12" t="s">

</xml_diff>